<commit_message>
change group by from lat long to id
</commit_message>
<xml_diff>
--- a/backend/PhotovoltaicSystemCalculation/PhotovoltaicSystemCalculation/EPreport.xlsx
+++ b/backend/PhotovoltaicSystemCalculation/PhotovoltaicSystemCalculation/EPreport.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Lat 52.521774 Long 13.351938" sheetId="1" r:id="rId1"/>
-    <sheet name="Lat 52.522243 Long 13.355005" sheetId="2" r:id="rId2"/>
+    <sheet name="Product ID  1 Hanwha Q-Cells" sheetId="1" r:id="rId1"/>
+    <sheet name="Product ID  2 First Solar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
cronjob working but still have duplicate bug
</commit_message>
<xml_diff>
--- a/backend/PhotovoltaicSystemCalculation/PhotovoltaicSystemCalculation/EPreport.xlsx
+++ b/backend/PhotovoltaicSystemCalculation/PhotovoltaicSystemCalculation/EPreport.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Product ID  1 Hanwha Q-Cells" sheetId="1" r:id="rId1"/>
-    <sheet name="Product ID  2 First Solar" sheetId="2" r:id="rId2"/>
+    <sheet name="Product ID 1 Hanwha Q-Cells" sheetId="1" r:id="rId1"/>
+    <sheet name="Product ID 2 First Solar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>